<commit_message>
fehlerhfate MPN Einträge geändert. Produktionsdaten ausgegeben
</commit_message>
<xml_diff>
--- a/Verstärker/BOM.xlsx
+++ b/Verstärker/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wks129_haw-hamburg_de/Documents/1HAW/1 Angewandte Elektronik/BOM Audioverstärker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nimai/KiCad/AEL/Verstärker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1076AC7E-772D-0E44-80D1-40AABA7E6C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD73833-5E13-C74B-95AE-69A3ABF2D699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="25600" windowHeight="16080" xr2:uid="{F315161E-6ABE-4A69-85A8-7E0F1B530356}"/>
+    <workbookView xWindow="15000" yWindow="660" windowWidth="13640" windowHeight="17180" xr2:uid="{F315161E-6ABE-4A69-85A8-7E0F1B530356}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
     <t>C17902</t>
   </si>
   <si>
-    <t>TO229P800X325X1420-3 (Bzw. TO220 in Kicad)</t>
+    <t>TO229P780X300X1364-3</t>
   </si>
 </sst>
 </file>
@@ -684,15 +684,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F1D5A6-F670-4C2C-8425-0AEBEFD5FFA3}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
@@ -835,258 +835,258 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1206</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1206</v>
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1206</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>510</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>200</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1206</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>75</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>510</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>200</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B36" s="1">
         <v>1206</v>
       </c>
-      <c r="C22">
+      <c r="C36">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D36" t="s">
         <v>66</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B37" s="1">
         <v>1206</v>
       </c>
-      <c r="C23">
+      <c r="C37">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D37" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E37" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1098,15 +1098,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008E5C6E5D804ABC43A8F1FCC5D1B85AA9" ma:contentTypeVersion="3" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="504c2aab5a80533b2f02dafd20b7e1ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b3639a0-2004-4b6d-b5e6-bbb93a920ad5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62fd73629e6d9c28fe4d1dbeb9e1917a" ns2:_="">
     <xsd:import namespace="9b3639a0-2004-4b6d-b5e6-bbb93a920ad5"/>
@@ -1244,15 +1235,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BE2DB9A-D24B-4B50-9F52-5F4139376813}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D5B3D4-222B-4040-9EF0-CA79F6661AC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1268,4 +1260,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BE2DB9A-D24B-4B50-9F52-5F4139376813}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>